<commit_message>
excel file path finding seperate func
</commit_message>
<xml_diff>
--- a/data/Portfell.xlsx
+++ b/data/Portfell.xlsx
@@ -332,7 +332,7 @@
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1533"/>
+  <dimension ref="A1:L1534"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -55388,6 +55388,46 @@
         <v>9341</v>
       </c>
     </row>
+    <row r="1534">
+      <c r="A1534" t="inlineStr">
+        <is>
+          <t>2025-03-29</t>
+        </is>
+      </c>
+      <c r="B1534" t="n">
+        <v>86016</v>
+      </c>
+      <c r="C1534" t="n">
+        <v>-3652</v>
+      </c>
+      <c r="D1534" t="n">
+        <v>97610</v>
+      </c>
+      <c r="E1534" t="n">
+        <v>93958</v>
+      </c>
+      <c r="F1534" t="n">
+        <v>179974</v>
+      </c>
+      <c r="G1534" t="n">
+        <v>120006</v>
+      </c>
+      <c r="H1534" t="n">
+        <v>309153</v>
+      </c>
+      <c r="I1534" t="n">
+        <v>109.31</v>
+      </c>
+      <c r="J1534" t="n">
+        <v>203</v>
+      </c>
+      <c r="K1534" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1534" t="n">
+        <v>9173</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="2"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Update stock values and portfolio calculations across multiple files
</commit_message>
<xml_diff>
--- a/data/Portfell.xlsx
+++ b/data/Portfell.xlsx
@@ -332,7 +332,7 @@
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1534"/>
+  <dimension ref="A1:L1535"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -55428,6 +55428,46 @@
         <v>9506</v>
       </c>
     </row>
+    <row r="1535">
+      <c r="A1535" t="inlineStr">
+        <is>
+          <t>2025-04-29</t>
+        </is>
+      </c>
+      <c r="B1535" t="n">
+        <v>118847.5</v>
+      </c>
+      <c r="C1535" t="n">
+        <v>-3753</v>
+      </c>
+      <c r="D1535" t="n">
+        <v>105186</v>
+      </c>
+      <c r="E1535" t="n">
+        <v>101433</v>
+      </c>
+      <c r="F1535" t="n">
+        <v>220280.5</v>
+      </c>
+      <c r="G1535" t="n">
+        <v>163879</v>
+      </c>
+      <c r="H1535" t="n">
+        <v>393458.5</v>
+      </c>
+      <c r="I1535" t="n">
+        <v>109.31</v>
+      </c>
+      <c r="J1535" t="n">
+        <v>1985</v>
+      </c>
+      <c r="K1535" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1535" t="n">
+        <v>9299</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="2"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
update: adjust portfolio values and loan balances for May 2025
</commit_message>
<xml_diff>
--- a/data/Portfell.xlsx
+++ b/data/Portfell.xlsx
@@ -337,7 +337,7 @@
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L1535"/>
+  <dimension ref="A1:L1536"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -55473,6 +55473,46 @@
         <v>9345</v>
       </c>
     </row>
+    <row r="1536">
+      <c r="A1536" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="B1536" t="n">
+        <v>87500</v>
+      </c>
+      <c r="C1536" t="n">
+        <v>-3675</v>
+      </c>
+      <c r="D1536" t="n">
+        <v>107799</v>
+      </c>
+      <c r="E1536" t="n">
+        <v>104124</v>
+      </c>
+      <c r="F1536" t="n">
+        <v>191624</v>
+      </c>
+      <c r="G1536" t="n">
+        <v>133788</v>
+      </c>
+      <c r="H1536" t="n">
+        <v>335112</v>
+      </c>
+      <c r="I1536" t="n">
+        <v>109.31</v>
+      </c>
+      <c r="J1536" t="n">
+        <v>2200</v>
+      </c>
+      <c r="K1536" t="n">
+        <v>4400</v>
+      </c>
+      <c r="L1536" t="n">
+        <v>9700</v>
+      </c>
+    </row>
     <row r="1538" ht="12.75" customHeight="1" s="1"/>
     <row r="1048564" ht="12.8" customHeight="1" s="1"/>
   </sheetData>

</xml_diff>